<commit_message>
merge Intel-Irris recent state
</commit_message>
<xml_diff>
--- a/Arduino/Osirris_Soil_Sensor/watermark.xlsx
+++ b/Arduino/Osirris_Soil_Sensor/watermark.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Dropbox (Compte personnel)/Arduino/sketch/00-PRIMA-Intel-Irris/Intelirris_Soil_Sensor/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpham/Library/CloudStorage/GoogleDrive-congduc.pham@waziup.org/Mon Drive/Arduino/sketch/00-PRIMA-Intel-Irris/Intelirris_Soil_Sensor/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A053E8-30A8-3C47-9357-FA53031BEB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1960" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="3180" yWindow="1940" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -65,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -183,6 +195,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -450,7 +465,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -471,7 +486,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="7">
-        <v>685</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -504,15 +519,15 @@
       </c>
       <c r="D5" s="2">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A5-24)))</f>
-        <v>2.0538599999999994</v>
+        <v>10.366864</v>
       </c>
       <c r="E5" s="2">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A5)))</f>
-        <v>9.5953489266611633</v>
+        <v>11.414668461720485</v>
       </c>
       <c r="F5" s="2">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A5-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A5-24))*(1+0.018*($A5-24))))</f>
-        <v>1.6375325792637443</v>
+        <v>3.7019425525458547</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -531,15 +546,15 @@
       </c>
       <c r="D6" s="4">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A6-24)))</f>
-        <v>2.1258599999999994</v>
+        <v>10.438863999999999</v>
       </c>
       <c r="E6" s="4">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A6)))</f>
-        <v>8.9385186300662749</v>
+        <v>10.629403556767031</v>
       </c>
       <c r="F6" s="4">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A6-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A6-24))*(1+0.018*($A6-24))))</f>
-        <v>1.374415841</v>
+        <v>3.2971520761600006</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
@@ -547,7 +562,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
-        <v>24.9</v>
+        <v>9</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>5</v>
@@ -558,15 +573,15 @@
       </c>
       <c r="D7" s="6">
         <f>ABS(($D$2/1000*23.156-12.736)-(1+0.018*($A7-24)))</f>
-        <v>2.1096599999999994</v>
+        <v>10.708863999999998</v>
       </c>
       <c r="E7" s="6">
         <f>ABS((-3.213*($D$2/1000)-4.093)/(1-0.009733*($D$2/1000)-0.01205*($A7)))</f>
-        <v>9.0783425549352774</v>
+        <v>8.4495882400350304</v>
       </c>
       <c r="F7" s="6">
         <f>ABS(2.246-5.239*($D$2/1000)*(1+0.018*($A7-24))-0.06756*($D$2/1000)*($D$2/1000)*((1+0.018*($A7-24))*(1+0.018*($A7-24))))</f>
-        <v>1.4335884508171122</v>
+        <v>1.7859873449856642</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>

</xml_diff>